<commit_message>
Update ER y MER
</commit_message>
<xml_diff>
--- a/docs/diagramas/ER.xlsx
+++ b/docs/diagramas/ER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inmun\source\repos\abadillo\bases-uno\docs\diagramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9C2577-AF3B-43EF-A881-435254D6A74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADE9D7D-F86D-4D6F-B492-B7DF05104220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-135" yWindow="105" windowWidth="21600" windowHeight="11415" xr2:uid="{F7C15000-705E-4203-8DC9-1952BB3143FD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="114">
   <si>
     <t xml:space="preserve"> 2. NN (Not Null)</t>
   </si>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035C990A-9B62-4EB6-A2FE-322E4C59F9D0}">
   <dimension ref="A1:L233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,13 +2024,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B129" s="2"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>6</v>
       </c>
@@ -2038,21 +2038,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B133" s="2"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>34</v>
       </c>
@@ -2060,14 +2060,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136" s="1"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>58</v>
       </c>
@@ -2077,15 +2078,19 @@
       <c r="C137" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138" s="2"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>6</v>
       </c>
@@ -2095,25 +2100,31 @@
       <c r="C139" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139" s="2"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" s="2"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" s="2"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>12</v>
       </c>
@@ -2121,6 +2132,9 @@
         <v>88</v>
       </c>
       <c r="C143" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D143" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2718,11 +2732,11 @@
     <mergeCell ref="A208:C208"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A217:E217"/>
+    <mergeCell ref="A136:D136"/>
     <mergeCell ref="A118:C118"/>
     <mergeCell ref="A127:B127"/>
     <mergeCell ref="A145:D145"/>
     <mergeCell ref="A172:C172"/>
-    <mergeCell ref="A136:C136"/>
     <mergeCell ref="A181:B181"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A73:C73"/>

</xml_diff>

<commit_message>
Update MER y ER
</commit_message>
<xml_diff>
--- a/docs/diagramas/ER.xlsx
+++ b/docs/diagramas/ER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\GitHub\bases-uno\docs\diagramas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inmun\source\repos\bases-uno\docs\diagramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C3D706-2877-4B26-B30E-F0647F79700C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF03508-C4AD-4F76-9CAC-1A17DAADF9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="107">
   <si>
     <t>CARACTERISTICAS</t>
   </si>
@@ -76,9 +76,6 @@
     <t>rol</t>
   </si>
   <si>
-    <t>id_sub</t>
-  </si>
-  <si>
     <t>Check ('Organizador', 'Invitado')</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>id_org</t>
   </si>
   <si>
-    <t>id_pre</t>
-  </si>
-  <si>
     <t>Check( mayor a 0 y menor o igual a 100 )</t>
   </si>
   <si>
@@ -344,13 +338,22 @@
   </si>
   <si>
     <t>precio_base_dollar</t>
+  </si>
+  <si>
+    <t>id_presencial</t>
+  </si>
+  <si>
+    <t>id_virtual</t>
+  </si>
+  <si>
+    <t>FK4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -403,6 +406,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -436,7 +445,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -533,6 +542,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -615,9 +637,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -633,6 +652,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,7 +663,35 @@
     <cellStyle name="Untitled3" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Untitled4" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF2A6099"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF2A6099"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <sz val="11"/>
@@ -1036,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1127,7 +1177,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1152,9 +1202,12 @@
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1166,15 +1219,17 @@
       <c r="C19" s="21" t="s">
         <v>12</v>
       </c>
+      <c r="D19" s="21" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="27"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1184,15 +1239,19 @@
         <v>13</v>
       </c>
       <c r="C21" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
@@ -1204,30 +1263,33 @@
       <c r="C23" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="D23" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:1024" s="3" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="AMJ26"/>
     </row>
@@ -1249,9 +1311,9 @@
       <c r="B28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="6" t="s">
         <v>4</v>
       </c>
@@ -1280,7 +1342,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>8</v>
@@ -1298,19 +1360,22 @@
     </row>
     <row r="33" spans="1:1024" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:1024" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>10</v>
       </c>
       <c r="AMJ34" s="7"/>
@@ -1325,16 +1390,18 @@
       <c r="C35" s="21" t="s">
         <v>12</v>
       </c>
+      <c r="D35" s="21" t="s">
+        <v>12</v>
+      </c>
       <c r="AMJ35" s="7"/>
     </row>
     <row r="36" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="27"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="6" t="s">
         <v>4</v>
       </c>
       <c r="AMJ36" s="7"/>
@@ -1344,10 +1411,13 @@
         <v>13</v>
       </c>
       <c r="B37" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="19" t="s">
-        <v>52</v>
+      <c r="D37" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="AMJ37" s="7"/>
     </row>
@@ -1355,6 +1425,7 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
       <c r="AMJ38" s="7"/>
     </row>
     <row r="39" spans="1:1024" x14ac:dyDescent="0.25">
@@ -1367,18 +1438,21 @@
       <c r="C39" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="D39" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="AMJ39" s="7"/>
     </row>
     <row r="41" spans="1:1024" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="9"/>
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>2</v>
@@ -1429,7 +1503,7 @@
     <row r="49" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:12" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1442,34 +1516,34 @@
     </row>
     <row r="51" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="G51" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="H51" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H51" s="4" t="s">
+      <c r="I51" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I51" s="4" t="s">
+      <c r="J51" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -1536,15 +1610,15 @@
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
       <c r="I55" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J55" s="6"/>
     </row>
@@ -1562,13 +1636,13 @@
         <v>7</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>8</v>
@@ -1577,7 +1651,7 @@
         <v>7</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -1587,45 +1661,45 @@
     </row>
     <row r="58" spans="1:12" s="7" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="D59" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="E59" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="F59" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="G59" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G59" s="4" t="s">
+      <c r="H59" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J59" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H59" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J59" s="4" t="s">
+      <c r="K59" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L59" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L59" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -1671,8 +1745,8 @@
       <c r="J61" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K61" s="28"/>
-      <c r="L61" s="30"/>
+      <c r="K61" s="27"/>
+      <c r="L61" s="29"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
@@ -1688,10 +1762,10 @@
         <v>13</v>
       </c>
       <c r="K62" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="L62" s="19" t="s">
         <v>51</v>
-      </c>
-      <c r="L62" s="19" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -1748,7 +1822,7 @@
     </row>
     <row r="66" spans="1:7" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1756,13 +1830,13 @@
     </row>
     <row r="67" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -1806,12 +1880,12 @@
     </row>
     <row r="74" spans="1:7" s="7" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>2</v>
@@ -1849,7 +1923,7 @@
     </row>
     <row r="82" spans="1:1024" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1857,19 +1931,19 @@
     </row>
     <row r="83" spans="1:1024" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AMJ83" s="13"/>
     </row>
@@ -1907,7 +1981,7 @@
         <v>13</v>
       </c>
       <c r="E86" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AMJ86"/>
     </row>
@@ -1927,7 +2001,7 @@
         <v>8</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>7</v>
@@ -1939,7 +2013,7 @@
     </row>
     <row r="90" spans="1:1024" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1947,16 +2021,16 @@
     </row>
     <row r="91" spans="1:1024" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C91" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="92" spans="1:1024" x14ac:dyDescent="0.25">
@@ -1991,7 +2065,7 @@
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D95" s="6"/>
     </row>
@@ -2017,15 +2091,15 @@
     </row>
     <row r="99" spans="1:1024" s="7" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:1024" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>15</v>
@@ -2034,7 +2108,7 @@
         <v>10</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AMJ100"/>
     </row>
@@ -2076,7 +2150,7 @@
         <v>13</v>
       </c>
       <c r="E103" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AMJ103"/>
     </row>
@@ -2084,7 +2158,7 @@
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D104" s="6"/>
       <c r="E104" s="6"/>
@@ -2092,10 +2166,10 @@
     </row>
     <row r="105" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>8</v>
@@ -2110,7 +2184,7 @@
     </row>
     <row r="107" spans="1:1024" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B107" s="7"/>
       <c r="C107" s="22"/>
@@ -2119,13 +2193,13 @@
     </row>
     <row r="108" spans="1:1024" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B108" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B108" s="14" t="s">
-        <v>68</v>
-      </c>
       <c r="C108" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AMI108"/>
       <c r="AMJ108"/>
@@ -2158,7 +2232,7 @@
         <v>13</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AMI111"/>
       <c r="AMJ111"/>
@@ -2185,16 +2259,16 @@
     </row>
     <row r="115" spans="1:1024" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B115" s="7"/>
     </row>
     <row r="116" spans="1:1024" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B116" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="117" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2218,7 +2292,7 @@
         <v>13</v>
       </c>
       <c r="B119" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="120" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2235,7 +2309,7 @@
     </row>
     <row r="123" spans="1:1024" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -2247,22 +2321,25 @@
     </row>
     <row r="124" spans="1:1024" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D124" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="E124" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="F124" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D124" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E124" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F124" s="4" t="s">
-        <v>68</v>
+      <c r="G124" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="AMJ124"/>
     </row>
@@ -2279,6 +2356,9 @@
       <c r="F125" s="21" t="s">
         <v>12</v>
       </c>
+      <c r="G125" s="21" t="s">
+        <v>3</v>
+      </c>
       <c r="AMJ125"/>
     </row>
     <row r="126" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2288,10 +2368,9 @@
         <v>4</v>
       </c>
       <c r="D126" s="6"/>
-      <c r="E126" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F126" s="6" t="s">
+      <c r="E126" s="27"/>
+      <c r="F126" s="29"/>
+      <c r="G126" s="6" t="s">
         <v>4</v>
       </c>
       <c r="AMJ126"/>
@@ -2305,23 +2384,27 @@
         <v>13</v>
       </c>
       <c r="F127" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G127" s="19" t="s">
         <v>51</v>
       </c>
       <c r="AMJ127"/>
     </row>
     <row r="128" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C128" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C128" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="D128" s="6"/>
       <c r="E128" s="27"/>
-      <c r="F128" s="27"/>
+      <c r="F128" s="28"/>
+      <c r="G128" s="32"/>
       <c r="AMJ128"/>
     </row>
     <row r="129" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2335,32 +2418,35 @@
         <v>7</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E129" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F129" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G129" s="6" t="s">
         <v>7</v>
       </c>
       <c r="AMJ129"/>
     </row>
     <row r="131" spans="1:1024" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
     </row>
     <row r="132" spans="1:1024" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B132" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B132" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="C132" s="4" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="133" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2389,12 +2475,12 @@
         <v>13</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="136" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B136" s="6"/>
       <c r="C136" s="6"/>
@@ -2412,19 +2498,19 @@
     </row>
     <row r="139" spans="1:1024" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B139" s="7"/>
     </row>
     <row r="140" spans="1:1024" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B140" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="141" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2466,7 +2552,7 @@
     </row>
     <row r="147" spans="1:1024" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
@@ -2480,13 +2566,13 @@
     </row>
     <row r="148" spans="1:1024" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AMJ148" s="7"/>
     </row>
@@ -2578,7 +2664,7 @@
     </row>
     <row r="155" spans="1:1024" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
@@ -2594,25 +2680,25 @@
     </row>
     <row r="156" spans="1:1024" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B156" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C156" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E156" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D156" s="4" t="s">
+      <c r="F156" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G156" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="E156" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F156" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G156" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="AMJ156"/>
     </row>
@@ -2687,11 +2773,11 @@
       <c r="B160" s="6"/>
       <c r="C160" s="6"/>
       <c r="D160" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E160" s="6"/>
       <c r="F160" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G160" s="6"/>
       <c r="AMD160" s="7"/>
@@ -2710,16 +2796,16 @@
         <v>8</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F161" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G161" s="6" t="s">
         <v>7</v>
@@ -2749,7 +2835,7 @@
     </row>
     <row r="163" spans="1:1024" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
@@ -2765,19 +2851,19 @@
     </row>
     <row r="164" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B164" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C164" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E164" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D164" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E164" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="165" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2842,7 +2928,7 @@
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
       <c r="D168" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E168" s="6"/>
       <c r="F168" s="7"/>
@@ -2862,13 +2948,13 @@
         <v>8</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D169" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F169" s="7"/>
       <c r="AMD169" s="7"/>
@@ -3667,13 +3753,27 @@
       <c r="AMJ256" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E128:F128"/>
+  <mergeCells count="6">
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="K61:L61"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E128:G128"/>
+    <mergeCell ref="E126:F126"/>
   </mergeCells>
-  <conditionalFormatting sqref="C26:AJ27 A106:A107 D123:AJ123 C24:C25 C32:C34 F86:AK86 C30 F30:AJ30 C29:AJ29 C28 F28:AJ28 D61:K61 M61:AK61 D1:AK25 B1:C23 B24:B34 C31:AJ31 A1:A34 A35:C39 D32:AK60 D62:AK85 D87:AK100 A40:A99 C40:C100 B101:C105 E101:AJ105 B40:B107 C106:AK122 F124:AJ129 D124:D129 C123:C129 C130:AK220 A114:B220">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="C26:AJ27 A106:A107 D123:AJ123 C24:C25 C32:C33 F86:AK86 C30 F30:AJ30 C29:AJ29 C28 F28:AJ28 D61:K61 M61:AK61 B1:C19 B24:B33 C31:AJ31 A1:A34 A35:C35 D62:AK85 D87:AK100 A40:A99 C40:C100 B101:C105 E101:AJ105 B40:B107 C106:AK122 D124:D129 C123:C129 C130:AK220 A114:B220 D1:AK25 B21:C23 B20 D32:AK60 A37:C39 A36:B36 F125:AJ125 F129:AJ129 H128:AJ128 F127:AJ127 G126:AJ126 G124:AJ124">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:C34">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E124:F124">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3696,34 +3796,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="A2" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>88</v>
-      </c>
       <c r="F3" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3769,11 +3869,11 @@
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3788,22 +3888,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="D9" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="F9" s="16" t="s">
         <v>98</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3812,30 +3912,30 @@
       <c r="C11" s="15"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
+      <c r="A13" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>86</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3876,7 +3976,7 @@
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="7"/>
@@ -3892,19 +3992,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="D20" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>97</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3916,33 +4016,33 @@
       <c r="F22"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
+      <c r="A32" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="18" t="s">
         <v>86</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -3988,10 +4088,10 @@
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
       <c r="D37" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F37" s="18"/>
     </row>
@@ -4007,22 +4107,22 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="D39" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>